<commit_message>
Add columns max_phase, first_approval
</commit_message>
<xml_diff>
--- a/supplements/targets/p_falciparum_hmmer_drugs.xlsx
+++ b/supplements/targets/p_falciparum_hmmer_drugs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeremy-satellite\Documents\RBIF120\paralog_targets\supplements\targets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FD4C819-D7EC-47B8-8A8E-E596EFF4B18F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{70A6AA5C-E0F6-4A64-806A-AAA22DB32743}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23130" yWindow="-3825" windowWidth="19410" windowHeight="10920"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="P_falciparum_hmmer_drugs" sheetId="1" r:id="rId1"/>
@@ -6036,13 +6036,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="33" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="36.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -6813,7 +6813,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>426.9</v>
       </c>
@@ -7189,7 +7189,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>533.70000000000005</v>
       </c>
@@ -7839,7 +7839,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>769.17499999999995</v>
       </c>
@@ -8028,7 +8028,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>426.9</v>
       </c>
@@ -8498,7 +8498,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>799.57500000000005</v>
       </c>
@@ -8805,7 +8805,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>769.17499999999995</v>
       </c>
@@ -10157,7 +10157,7 @@
         <v>1957</v>
       </c>
     </row>
-    <row r="191" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>457.57499999999999</v>
       </c>
@@ -10203,7 +10203,7 @@
         <v>1967</v>
       </c>
     </row>
-    <row r="193" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>1063.8571428571399</v>
       </c>
@@ -10699,7 +10699,7 @@
         <v>1979</v>
       </c>
     </row>
-    <row r="216" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>411.9</v>
       </c>
@@ -10894,7 +10894,7 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="225" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>475.5</v>
       </c>
@@ -11089,7 +11089,7 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="234" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>1063.8571428571399</v>
       </c>
@@ -11293,7 +11293,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="243" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>500.77692307692303</v>
       </c>
@@ -11382,7 +11382,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="247" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>426.9</v>
       </c>
@@ -11563,7 +11563,7 @@
         <v>1991</v>
       </c>
     </row>
-    <row r="255" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>426.9</v>
       </c>
@@ -11586,7 +11586,7 @@
         <v>1959</v>
       </c>
     </row>
-    <row r="256" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>1085.2166666666601</v>
       </c>
@@ -11609,7 +11609,7 @@
         <v>1946</v>
       </c>
     </row>
-    <row r="257" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>1063.8571428571399</v>
       </c>
@@ -12722,7 +12722,7 @@
         <v>1967</v>
       </c>
     </row>
-    <row r="308" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>1063.8571428571399</v>
       </c>
@@ -12877,7 +12877,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="315" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>661.12</v>
       </c>
@@ -13264,7 +13264,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="333" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>1085.2166666666601</v>
       </c>
@@ -14098,7 +14098,7 @@
         <v>1969</v>
       </c>
     </row>
-    <row r="372" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A372">
         <v>553.9</v>
       </c>
@@ -14844,7 +14844,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="406" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A406">
         <v>638.9</v>
       </c>
@@ -14867,7 +14867,7 @@
         <v>1966</v>
       </c>
     </row>
-    <row r="407" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A407">
         <v>638.9</v>
       </c>
@@ -14936,7 +14936,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="410" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A410">
         <v>638.9</v>
       </c>
@@ -15051,7 +15051,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="415" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A415">
         <v>638.9</v>
       </c>
@@ -15120,7 +15120,7 @@
         <v>1987</v>
       </c>
     </row>
-    <row r="418" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A418">
         <v>638.9</v>
       </c>
@@ -15166,7 +15166,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="420" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A420">
         <v>638.9</v>
       </c>
@@ -15212,7 +15212,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="422" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A422">
         <v>638.9</v>
       </c>
@@ -15258,7 +15258,7 @@
         <v>1985</v>
       </c>
     </row>
-    <row r="424" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A424">
         <v>638.9</v>
       </c>
@@ -15929,7 +15929,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="455" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A455">
         <v>426.9</v>
       </c>
@@ -16038,7 +16038,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="460" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A460">
         <v>426.9</v>
       </c>
@@ -16651,7 +16651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="489" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A489">
         <v>1063.8571428571399</v>
       </c>
@@ -16674,7 +16674,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="490" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A490">
         <v>553.9</v>
       </c>
@@ -16924,7 +16924,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="501" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A501">
         <v>1063.8571428571399</v>
       </c>
@@ -16947,7 +16947,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="502" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A502">
         <v>710.9</v>
       </c>
@@ -17128,7 +17128,7 @@
         <v>1955</v>
       </c>
     </row>
-    <row r="510" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A510">
         <v>426.9</v>
       </c>
@@ -17151,7 +17151,7 @@
         <v>1955</v>
       </c>
     </row>
-    <row r="511" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A511">
         <v>715.65</v>
       </c>
@@ -18522,7 +18522,7 @@
         <v>1968</v>
       </c>
     </row>
-    <row r="574" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="574" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A574">
         <v>426.9</v>
       </c>
@@ -18849,7 +18849,7 @@
         <v>1959</v>
       </c>
     </row>
-    <row r="589" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="589" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A589">
         <v>426.9</v>
       </c>
@@ -19004,7 +19004,7 @@
         <v>1983</v>
       </c>
     </row>
-    <row r="596" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="596" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A596">
         <v>548.75</v>
       </c>
@@ -19073,7 +19073,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="599" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="599" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A599">
         <v>1063.8571428571399</v>
       </c>
@@ -19828,7 +19828,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="633" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="633" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A633">
         <v>426.9</v>
       </c>
@@ -19851,7 +19851,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="634" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="634" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A634">
         <v>548.75</v>
       </c>
@@ -20012,7 +20012,7 @@
         <v>1958</v>
       </c>
     </row>
-    <row r="641" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="641" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A641">
         <v>426.9</v>
       </c>
@@ -20379,7 +20379,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="658" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="658" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A658">
         <v>533.70000000000005</v>
       </c>
@@ -20594,7 +20594,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="668" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="668" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A668">
         <v>715.65</v>
       </c>
@@ -20617,7 +20617,7 @@
         <v>1989</v>
       </c>
     </row>
-    <row r="669" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="669" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A669">
         <v>715.65</v>
       </c>
@@ -20686,7 +20686,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="672" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="672" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A672">
         <v>426.9</v>
       </c>
@@ -20749,7 +20749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="675" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="675" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A675">
         <v>426.9</v>
       </c>
@@ -22191,7 +22191,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="742" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="742" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A742">
         <v>1063.8571428571399</v>
       </c>
@@ -22839,7 +22839,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="772" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="772" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A772">
         <v>615.5</v>
       </c>
@@ -22862,7 +22862,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="773" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="773" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A773">
         <v>615.5</v>
       </c>
@@ -23083,7 +23083,7 @@
         <v>1953</v>
       </c>
     </row>
-    <row r="783" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="783" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A783">
         <v>1063.8571428571399</v>
       </c>
@@ -23106,7 +23106,7 @@
         <v>1957</v>
       </c>
     </row>
-    <row r="784" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="784" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A784">
         <v>548.75</v>
       </c>
@@ -23528,7 +23528,7 @@
         <v>1985</v>
       </c>
     </row>
-    <row r="803" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="803" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A803">
         <v>408.4</v>
       </c>
@@ -23663,7 +23663,7 @@
         <v>1971</v>
       </c>
     </row>
-    <row r="809" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="809" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A809">
         <v>457.57499999999999</v>
       </c>
@@ -24575,5 +24575,6 @@
   </sheetData>
   <autoFilter ref="A1:G850"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>